<commit_message>
new waves and enemies
</commit_message>
<xml_diff>
--- a/enemyType.xlsx
+++ b/enemyType.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="121">
   <si>
     <t>Color</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -225,157 +225,246 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>large, randomFiring</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mineLayer</t>
+  </si>
+  <si>
+    <t>indestructibleFiring</t>
+  </si>
+  <si>
+    <t>aimedFiring, counterAttack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bulletAttractor</t>
+  </si>
+  <si>
+    <t>attract</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>repel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bulletRepulsor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>aimFire, closeIn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>generator</t>
+  </si>
+  <si>
+    <t>generate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sneaky</t>
+  </si>
+  <si>
+    <t>view, aimedFire</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sneaky</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stay, slow, view</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mineLayer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bulletSneaky</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fastRandomFiring</t>
+  </si>
+  <si>
+    <t>fast, frequentRandomFiring</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hp, aimedFiring, randomFiring3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fireChasing</t>
+  </si>
+  <si>
+    <t>fireChase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>darkFiring</t>
+  </si>
+  <si>
+    <t>dark</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>autoTeleporting</t>
+  </si>
+  <si>
+    <t>teleporting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>splitRandomFiring</t>
+  </si>
+  <si>
+    <t>split</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>splitTo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30/12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fastRandomFiring, hp, aimedFiring</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hpSmallChasing</t>
+  </si>
+  <si>
+    <t>smallChasing, hp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>moveForceToPlayer</t>
+  </si>
+  <si>
+    <t>forceToPlayer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hpIndestructibleCounterAttack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>move</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>counterAttack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3/10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chaserGenerator</t>
+  </si>
+  <si>
+    <t>aimFire</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>generator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chasing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>immuneUntilTargetBeaten</t>
+  </si>
+  <si>
+    <t>&lt;8&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>immuneUntilTarget</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>burstBullet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>move, aimFire</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hp, aimedFiring</t>
+  </si>
+  <si>
+    <t>12/72</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3/5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>attractCounterAttack</t>
+  </si>
+  <si>
+    <t>attractor, counterAttack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>repelAimedFiring</t>
+  </si>
+  <si>
+    <t>hpAimedFiring3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>repulsor, hpAimedFiring3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>aimFire, view</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>spreadFire</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>view, move</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>transparentFiring</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>largeFiring</t>
-  </si>
-  <si>
-    <t>large, randomFiring</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mineLayer</t>
-  </si>
-  <si>
-    <t>indestructibleFiring</t>
-  </si>
-  <si>
-    <t>aimedFiring, counterAttack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bulletAttractor</t>
-  </si>
-  <si>
-    <t>attract</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>repel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bulletRepulsor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>aimFire, closeIn</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>generator</t>
-  </si>
-  <si>
-    <t>generate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sneaky</t>
-  </si>
-  <si>
-    <t>view, aimedFire</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sneaky</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>burstOnHit</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>sneakyMineLayer</t>
-  </si>
-  <si>
-    <t>stay, slow, view</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mineLayer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bulletSneaky</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fastRandomFiring</t>
-  </si>
-  <si>
-    <t>fast, frequentRandomFiring</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hpAimedFiring3</t>
-  </si>
-  <si>
-    <t>hp, aimedFiring, randomFiring3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fireChasing</t>
-  </si>
-  <si>
-    <t>fireChase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>darkFiring</t>
-  </si>
-  <si>
-    <t>dark</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>autoTeleporting</t>
-  </si>
-  <si>
-    <t>teleporting</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>teleportFiring</t>
-  </si>
-  <si>
-    <t>stay, move</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>teleporting, aimedFiring</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>splitRandomFiring</t>
-  </si>
-  <si>
-    <t>split</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>splitTo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>burstOnHit</t>
-  </si>
-  <si>
-    <t>30/12</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>hpFastAimedFiring</t>
-  </si>
-  <si>
-    <t>fastRandomFiring, hp, aimedFiring</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hpSmallChasing</t>
-  </si>
-  <si>
-    <t>smallChasing, hp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>moveForceToPlayer</t>
-  </si>
-  <si>
-    <t>forceToPlayer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>frequentAimedFiring</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -400,7 +489,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="40">
+  <fills count="47">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -601,12 +690,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFBF86E"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC2470A"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -632,6 +715,54 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF01FF56"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4AF24"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0DF35A"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF01FF80"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF71FF80"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF01FFD5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF01FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF01CFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF01AAFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -650,7 +781,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -769,6 +900,27 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -779,16 +931,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FF01FF56"/>
-      <color rgb="FFC2290A"/>
-      <color rgb="FFCC6734"/>
-      <color rgb="FFF3A60D"/>
-      <color rgb="FFC2470A"/>
-      <color rgb="FFFBF86E"/>
-      <color rgb="FFFFFF67"/>
-      <color rgb="FF331201"/>
-      <color rgb="FF01FF2B"/>
-      <color rgb="FFEB9947"/>
+      <color rgb="FF01AAFF"/>
+      <color rgb="FFF3CD0D"/>
+      <color rgb="FF01CFFF"/>
+      <color rgb="FF01FFFF"/>
+      <color rgb="FF01FFD5"/>
+      <color rgb="FF71FF80"/>
+      <color rgb="FF01FF80"/>
+      <color rgb="FF0DF35A"/>
+      <color rgb="FF2BE601"/>
+      <color rgb="FFF4AF24"/>
     </mruColors>
   </colors>
 </styleSheet>
@@ -1079,19 +1231,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB39"/>
+  <dimension ref="A1:AC46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E38" sqref="E38"/>
+      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="5.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.375" bestFit="1" customWidth="1"/>
@@ -1104,7 +1256,7 @@
     <col min="12" max="12" width="8.25" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.5" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="7.375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="6" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11.875" bestFit="1" customWidth="1"/>
@@ -1115,9 +1267,11 @@
     <col min="26" max="26" width="4.75" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="12.375" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:29">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1176,40 +1330,43 @@
         <v>43</v>
       </c>
       <c r="T1" t="s">
+        <v>61</v>
+      </c>
+      <c r="U1" t="s">
         <v>62</v>
       </c>
-      <c r="U1" t="s">
-        <v>63</v>
-      </c>
       <c r="V1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="W1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="X1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="Y1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="Z1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="AA1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB1" t="s">
         <v>90</v>
       </c>
-      <c r="AB1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28">
+      <c r="AC1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:29">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
         <v>7</v>
@@ -1218,7 +1375,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:29">
       <c r="A4" s="3"/>
       <c r="B4" t="s">
         <v>9</v>
@@ -1236,7 +1393,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:29">
       <c r="A5" s="4"/>
       <c r="B5" t="s">
         <v>13</v>
@@ -1263,7 +1420,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:29">
       <c r="A6" s="5"/>
       <c r="B6" t="s">
         <v>16</v>
@@ -1275,7 +1432,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:28">
+    <row r="7" spans="1:29">
       <c r="A7" s="6"/>
       <c r="B7" t="s">
         <v>18</v>
@@ -1305,7 +1462,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:28">
+    <row r="8" spans="1:29">
       <c r="A8" s="7"/>
       <c r="B8" t="s">
         <v>19</v>
@@ -1320,7 +1477,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:28">
+    <row r="9" spans="1:29">
       <c r="A9" s="8"/>
       <c r="B9" t="s">
         <v>20</v>
@@ -1329,7 +1486,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="10" spans="1:28">
+    <row r="10" spans="1:29">
       <c r="A10" s="9"/>
       <c r="B10" t="s">
         <v>21</v>
@@ -1338,7 +1495,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:28">
+    <row r="11" spans="1:29">
       <c r="A11" s="10"/>
       <c r="B11" t="s">
         <v>24</v>
@@ -1365,7 +1522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:28">
+    <row r="12" spans="1:29">
       <c r="A12" s="11"/>
       <c r="B12" t="s">
         <v>26</v>
@@ -1395,7 +1552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:28">
+    <row r="13" spans="1:29">
       <c r="A13" s="12"/>
       <c r="B13" t="s">
         <v>28</v>
@@ -1413,7 +1570,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:28">
+    <row r="14" spans="1:29">
       <c r="A14" s="13"/>
       <c r="B14" t="s">
         <v>32</v>
@@ -1431,7 +1588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:28">
+    <row r="15" spans="1:29">
       <c r="A15" s="15"/>
       <c r="B15" t="s">
         <v>34</v>
@@ -1458,7 +1615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:28">
+    <row r="16" spans="1:29">
       <c r="A16" s="16"/>
       <c r="B16" t="s">
         <v>37</v>
@@ -1572,13 +1729,13 @@
     <row r="21" spans="1:25">
       <c r="A21" s="21"/>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="C21">
         <v>0.4</v>
       </c>
       <c r="F21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H21">
         <v>100</v>
@@ -1599,7 +1756,7 @@
     <row r="22" spans="1:25">
       <c r="A22" s="22"/>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E22" t="s">
         <v>36</v>
@@ -1620,13 +1777,13 @@
     <row r="23" spans="1:25">
       <c r="A23" s="23"/>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E23" t="s">
         <v>22</v>
       </c>
       <c r="F23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H23">
         <v>100</v>
@@ -1650,7 +1807,7 @@
     <row r="24" spans="1:25">
       <c r="A24" s="24"/>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E24" t="s">
         <v>23</v>
@@ -1658,26 +1815,26 @@
       <c r="O24">
         <v>20</v>
       </c>
-      <c r="T24" t="b">
-        <v>1</v>
+      <c r="T24">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="25" spans="1:25">
       <c r="A25" s="25"/>
       <c r="B25" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" t="s">
         <v>64</v>
       </c>
-      <c r="E25" t="s">
-        <v>65</v>
-      </c>
-      <c r="U25" t="b">
-        <v>1</v>
+      <c r="U25">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="26" spans="1:25">
       <c r="A26" s="26"/>
       <c r="B26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E26" t="s">
         <v>23</v>
@@ -1698,10 +1855,10 @@
     <row r="27" spans="1:25">
       <c r="A27" s="27"/>
       <c r="B27" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" t="s">
         <v>68</v>
-      </c>
-      <c r="E27" t="s">
-        <v>69</v>
       </c>
       <c r="F27" t="s">
         <v>8</v>
@@ -1716,13 +1873,13 @@
     <row r="28" spans="1:25">
       <c r="A28" s="28"/>
       <c r="B28" t="s">
+        <v>118</v>
+      </c>
+      <c r="E28" t="s">
+        <v>70</v>
+      </c>
+      <c r="F28" t="s">
         <v>71</v>
-      </c>
-      <c r="E28" t="s">
-        <v>72</v>
-      </c>
-      <c r="F28" t="s">
-        <v>73</v>
       </c>
       <c r="H28">
         <v>50</v>
@@ -1743,13 +1900,13 @@
     <row r="29" spans="1:25">
       <c r="A29" s="29"/>
       <c r="B29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D29">
         <v>6</v>
       </c>
       <c r="F29" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H29">
         <v>40</v>
@@ -1767,13 +1924,13 @@
     <row r="30" spans="1:25">
       <c r="A30" s="30"/>
       <c r="B30" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="E30" t="s">
         <v>35</v>
       </c>
       <c r="F30" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H30">
         <v>100</v>
@@ -1800,7 +1957,7 @@
     <row r="31" spans="1:25">
       <c r="A31" s="31"/>
       <c r="B31" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E31" t="s">
         <v>22</v>
@@ -1827,10 +1984,10 @@
     <row r="32" spans="1:25">
       <c r="A32" s="32"/>
       <c r="B32" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E32" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F32" t="s">
         <v>45</v>
@@ -1848,16 +2005,16 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:28">
+    <row r="33" spans="1:29">
       <c r="A33" s="33"/>
       <c r="B33" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E33" t="s">
         <v>36</v>
       </c>
       <c r="F33" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="O33">
         <v>5</v>
@@ -1866,19 +2023,16 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:28">
+    <row r="34" spans="1:29">
       <c r="A34" s="34"/>
       <c r="B34" t="s">
-        <v>85</v>
-      </c>
-      <c r="E34" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F34" t="s">
-        <v>87</v>
+        <v>45</v>
       </c>
       <c r="H34">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="I34">
         <v>5</v>
@@ -1889,26 +2043,23 @@
       <c r="K34">
         <v>60</v>
       </c>
-      <c r="N34">
-        <v>10</v>
-      </c>
-      <c r="O34">
-        <v>3</v>
-      </c>
-      <c r="Q34">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="35" spans="1:28">
+      <c r="Z34">
+        <v>9</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29">
       <c r="A35" s="35"/>
       <c r="B35" t="s">
-        <v>88</v>
+        <v>117</v>
+      </c>
+      <c r="E35" t="s">
+        <v>35</v>
       </c>
       <c r="F35" t="s">
-        <v>45</v>
-      </c>
-      <c r="H35">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="I35">
         <v>5</v>
@@ -1919,44 +2070,50 @@
       <c r="K35">
         <v>60</v>
       </c>
-      <c r="Z35">
-        <v>9</v>
-      </c>
-      <c r="AA35" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:28">
-      <c r="A36" s="36"/>
+      <c r="M35" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="P35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29">
+      <c r="A36" s="39"/>
       <c r="B36" t="s">
         <v>91</v>
       </c>
       <c r="E36" t="s">
-        <v>35</v>
+        <v>92</v>
       </c>
       <c r="F36" t="s">
-        <v>24</v>
-      </c>
-      <c r="I36">
-        <v>5</v>
-      </c>
-      <c r="J36">
-        <v>0.06</v>
+        <v>93</v>
       </c>
       <c r="K36">
-        <v>60</v>
+        <v>100</v>
+      </c>
+      <c r="L36" t="b">
+        <v>1</v>
       </c>
       <c r="M36" s="14" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="N36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:28">
-      <c r="A37" s="37"/>
+      <c r="O36">
+        <v>5</v>
+      </c>
+      <c r="P36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29">
+      <c r="A37" s="36"/>
       <c r="B37" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="D37">
         <v>6</v>
@@ -1965,7 +2122,7 @@
         <v>22</v>
       </c>
       <c r="F37" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="H37">
         <v>40</v>
@@ -1986,10 +2143,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:28">
-      <c r="A38" s="38"/>
+    <row r="38" spans="1:29">
+      <c r="A38" s="37"/>
       <c r="B38" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C38">
         <v>0.04</v>
@@ -1998,7 +2155,7 @@
         <v>22</v>
       </c>
       <c r="F38" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="G38">
         <v>0.06</v>
@@ -2007,10 +2164,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:28">
-      <c r="A39" s="39"/>
+    <row r="39" spans="1:29">
+      <c r="A39" s="38"/>
       <c r="B39" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E39" t="s">
         <v>22</v>
@@ -2023,6 +2180,219 @@
       </c>
       <c r="AB39">
         <v>0.01</v>
+      </c>
+    </row>
+    <row r="40" spans="1:29">
+      <c r="A40" s="40"/>
+      <c r="B40" t="s">
+        <v>95</v>
+      </c>
+      <c r="E40" t="s">
+        <v>96</v>
+      </c>
+      <c r="F40" t="s">
+        <v>97</v>
+      </c>
+      <c r="H40">
+        <v>100</v>
+      </c>
+      <c r="O40">
+        <v>8</v>
+      </c>
+      <c r="V40" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:29">
+      <c r="A41" s="41"/>
+      <c r="B41" t="s">
+        <v>99</v>
+      </c>
+      <c r="E41" t="s">
+        <v>112</v>
+      </c>
+      <c r="F41" t="s">
+        <v>104</v>
+      </c>
+      <c r="H41">
+        <v>50</v>
+      </c>
+      <c r="I41">
+        <v>5</v>
+      </c>
+      <c r="J41">
+        <v>0.06</v>
+      </c>
+      <c r="K41">
+        <v>60</v>
+      </c>
+      <c r="O41" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:29">
+      <c r="A42" s="42"/>
+      <c r="B42" t="s">
+        <v>102</v>
+      </c>
+      <c r="E42" t="s">
+        <v>103</v>
+      </c>
+      <c r="F42" t="s">
+        <v>104</v>
+      </c>
+      <c r="H42">
+        <v>50</v>
+      </c>
+      <c r="I42" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="J42">
+        <v>0.06</v>
+      </c>
+      <c r="K42">
+        <v>60</v>
+      </c>
+      <c r="M42" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="O42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:29">
+      <c r="A43" s="43"/>
+      <c r="B43" t="s">
+        <v>107</v>
+      </c>
+      <c r="E43" t="s">
+        <v>103</v>
+      </c>
+      <c r="F43" t="s">
+        <v>108</v>
+      </c>
+      <c r="I43">
+        <v>5</v>
+      </c>
+      <c r="J43">
+        <v>0.06</v>
+      </c>
+      <c r="K43">
+        <v>100</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
+      </c>
+      <c r="O43">
+        <v>30</v>
+      </c>
+      <c r="P43" t="b">
+        <v>1</v>
+      </c>
+      <c r="T43">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:29">
+      <c r="A44" s="44"/>
+      <c r="B44" t="s">
+        <v>109</v>
+      </c>
+      <c r="E44" t="s">
+        <v>64</v>
+      </c>
+      <c r="F44" t="s">
+        <v>111</v>
+      </c>
+      <c r="H44">
+        <v>100</v>
+      </c>
+      <c r="I44">
+        <v>5</v>
+      </c>
+      <c r="J44">
+        <v>0.06</v>
+      </c>
+      <c r="K44">
+        <v>60</v>
+      </c>
+      <c r="M44" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <v>3</v>
+      </c>
+      <c r="U44">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:29">
+      <c r="A45" s="45"/>
+      <c r="B45" t="s">
+        <v>120</v>
+      </c>
+      <c r="E45" t="s">
+        <v>113</v>
+      </c>
+      <c r="F45" t="s">
+        <v>45</v>
+      </c>
+      <c r="H45">
+        <v>33</v>
+      </c>
+      <c r="I45">
+        <v>5</v>
+      </c>
+      <c r="J45">
+        <v>0.06</v>
+      </c>
+      <c r="K45">
+        <v>60</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:29">
+      <c r="A46" s="46"/>
+      <c r="B46" t="s">
+        <v>115</v>
+      </c>
+      <c r="E46" t="s">
+        <v>114</v>
+      </c>
+      <c r="F46" t="s">
+        <v>110</v>
+      </c>
+      <c r="G46">
+        <v>0.06</v>
+      </c>
+      <c r="H46">
+        <v>100</v>
+      </c>
+      <c r="I46">
+        <v>5</v>
+      </c>
+      <c r="J46">
+        <v>0.06</v>
+      </c>
+      <c r="K46">
+        <v>60</v>
+      </c>
+      <c r="M46" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+      <c r="O46">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>